<commit_message>
introduces weight diff > 0.75 instead of expected reward > 0.5 for bg loop training
</commit_message>
<xml_diff>
--- a/StatisticalAnalysis/01_Exp_BG_Training_Iterations.xlsx
+++ b/StatisticalAnalysis/01_Exp_BG_Training_Iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geige\Documents\MasterThesisCode\SpikingLearningModel\StatisticalAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1081D5EA-2F93-4EAC-A6D1-9FF08868AB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC26FE5-1E0C-4963-A474-07D9CB34F4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="12">
   <si>
     <t>Experiment</t>
   </si>
@@ -68,10 +68,10 @@
     <t>GroupName</t>
   </si>
   <si>
-    <t>Exoskeleton (opposition sensor at actuator)</t>
-  </si>
-  <si>
-    <t>Exoskeleton (opposition sensor between fingers)</t>
+    <t>Experiment (opposition sensor at actuator)</t>
+  </si>
+  <si>
+    <t>Experiment (opposition sensor between fingers)</t>
   </si>
 </sst>
 </file>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -472,7 +472,7 @@
         <v>468</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G21" si="0">F3-E3</f>
+        <f t="shared" ref="G3:G23" si="0">F3-E3</f>
         <v>54</v>
       </c>
     </row>
@@ -625,13 +625,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -640,36 +640,36 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
-        <v>325</v>
+        <f t="shared" ref="G10:G11" si="1">F10-E10</f>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11">
         <f>F10</f>
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="F11">
-        <v>381</v>
+        <v>410</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -680,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -689,11 +689,11 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>401</v>
+        <v>325</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>401</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -704,21 +704,21 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13">
         <f>F12</f>
-        <v>401</v>
+        <v>325</v>
       </c>
       <c r="F13">
-        <v>515</v>
+        <v>381</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -729,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -738,11 +738,11 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>372</v>
+        <v>401</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>372</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -753,21 +753,21 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15">
         <f>F14</f>
-        <v>372</v>
+        <v>401</v>
       </c>
       <c r="F15">
-        <v>490</v>
+        <v>515</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -787,11 +787,11 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -802,21 +802,21 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17">
         <f>F16</f>
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F17">
-        <v>405</v>
+        <v>490</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -836,11 +836,11 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G19" si="1">F18-E18</f>
-        <v>381</v>
+        <f t="shared" si="0"/>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -851,32 +851,32 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19">
         <f>F18</f>
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F19">
-        <v>462</v>
+        <v>405</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>81</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -884,29 +884,78 @@
       <c r="E20">
         <v>0</v>
       </c>
+      <c r="F20">
+        <v>381</v>
+      </c>
       <c r="G20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="G20:G21" si="2">F20-E20</f>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21">
         <f>F20</f>
-        <v>0</v>
+        <v>381</v>
+      </c>
+      <c r="F21">
+        <v>462</v>
       </c>
       <c r="G21">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <f>F22</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>